<commit_message>
helper fx to create file description
</commit_message>
<xml_diff>
--- a/data/1tableoftables.xlsx
+++ b/data/1tableoftables.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>name</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>gpl3</t>
+  </si>
+  <si>
+    <t>AJS_AmTiman_population</t>
   </si>
   <si>
     <t>population</t>
@@ -819,11 +822,11 @@
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" t="s">
-        <v>15</v>
+      <c r="A3" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -856,7 +859,7 @@
         <v>2016</v>
       </c>
       <c r="M3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N3" t="s">
         <v>26</v>
@@ -867,13 +870,13 @@
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
@@ -903,7 +906,7 @@
         <v>2016</v>
       </c>
       <c r="M4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N4" t="s">
         <v>26</v>
@@ -914,13 +917,13 @@
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
@@ -950,7 +953,7 @@
         <v>2016</v>
       </c>
       <c r="M5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>26</v>
@@ -961,16 +964,16 @@
     </row>
     <row r="6" ht="14.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E6" s="6">
         <v>1</v>
@@ -979,25 +982,25 @@
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L6" s="3">
         <v>2021</v>
       </c>
       <c r="M6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N6" t="s">
         <v>26</v>
@@ -1008,16 +1011,16 @@
     </row>
     <row r="7" ht="14.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E7" s="6">
         <v>1</v>
@@ -1026,25 +1029,25 @@
         <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L7">
         <v>2021</v>
       </c>
       <c r="M7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N7" t="s">
         <v>26</v>

</xml_diff>